<commit_message>
main test and recon test
</commit_message>
<xml_diff>
--- a/tests/test2_calc.xlsx
+++ b/tests/test2_calc.xlsx
@@ -9,12 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-27180" yWindow="-10000" windowWidth="28800" windowHeight="17560" tabRatio="500"/>
+    <workbookView xWindow="-38400" yWindow="-11860" windowWidth="28440" windowHeight="21600" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="22">
   <si>
     <t>D0-POS</t>
   </si>
@@ -84,6 +84,15 @@
   </si>
   <si>
     <t>Cash Amt</t>
+  </si>
+  <si>
+    <t>Changes</t>
+  </si>
+  <si>
+    <t>Beg Cash</t>
+  </si>
+  <si>
+    <t>End Cash</t>
   </si>
 </sst>
 </file>
@@ -92,9 +101,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -117,8 +126,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -155,8 +172,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -193,12 +216,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -215,8 +247,19 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="43" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="5" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="0" fillId="6" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="43" fontId="3" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -495,10 +538,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L12"/>
+  <dimension ref="A1:M14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="216" zoomScaleNormal="216" zoomScalePageLayoutView="216" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2:I11"/>
+    <sheetView tabSelected="1" zoomScale="216" zoomScaleNormal="216" zoomScalePageLayoutView="216" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -513,9 +556,10 @@
     <col min="8" max="8" width="10" style="1" customWidth="1"/>
     <col min="9" max="9" width="7.5" style="1" customWidth="1"/>
     <col min="10" max="10" width="4.33203125" customWidth="1"/>
+    <col min="12" max="12" width="1.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -538,11 +582,11 @@
       <c r="K1" t="s">
         <v>16</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
         <v>3</v>
       </c>
@@ -579,12 +623,13 @@
         <f>B2+E2*J2</f>
         <v>589</v>
       </c>
-      <c r="L2" s="10">
+      <c r="L2" s="10"/>
+      <c r="M2" s="10">
         <f>-J2*F2</f>
         <v>-1430</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
         <v>5</v>
       </c>
@@ -610,7 +655,7 @@
         <v>1298.75</v>
       </c>
       <c r="I3" s="14">
-        <f t="shared" ref="I3:I10" si="0">H3-K3</f>
+        <f t="shared" ref="I3:I9" si="0">H3-K3</f>
         <v>0</v>
       </c>
       <c r="J3">
@@ -621,12 +666,13 @@
         <f t="shared" ref="K3:K10" si="1">B3+E3*J3</f>
         <v>1298.75</v>
       </c>
-      <c r="L3" s="10">
+      <c r="L3" s="10"/>
+      <c r="M3" s="10">
         <f>-J3*F3</f>
         <v>-3194</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
         <v>13</v>
       </c>
@@ -648,12 +694,13 @@
         <f t="shared" si="1"/>
         <v>1020</v>
       </c>
-      <c r="L4" s="10">
+      <c r="L4" s="10"/>
+      <c r="M4" s="10">
         <f>-J4*F4</f>
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" s="9" t="s">
         <v>6</v>
       </c>
@@ -690,12 +737,13 @@
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
-      <c r="L5" s="10">
+      <c r="L5" s="10"/>
+      <c r="M5" s="10">
         <f>-J5*F5</f>
         <v>3412</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" s="9" t="s">
         <v>14</v>
       </c>
@@ -717,12 +765,13 @@
         <f t="shared" si="1"/>
         <v>123</v>
       </c>
-      <c r="L6" s="10">
+      <c r="L6" s="10"/>
+      <c r="M6" s="10">
         <f>-J6*F6</f>
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" s="9" t="s">
         <v>8</v>
       </c>
@@ -759,12 +808,13 @@
         <f t="shared" si="1"/>
         <v>318</v>
       </c>
-      <c r="L7" s="10">
+      <c r="L7" s="10"/>
+      <c r="M7" s="10">
         <f>-J7*F7</f>
         <v>140</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" s="9" t="s">
         <v>9</v>
       </c>
@@ -801,12 +851,13 @@
         <f t="shared" si="1"/>
         <v>584</v>
       </c>
-      <c r="L8" s="10">
+      <c r="L8" s="10"/>
+      <c r="M8" s="10">
         <f>-J8*F8</f>
         <v>-4323</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" s="9" t="s">
         <v>15</v>
       </c>
@@ -828,12 +879,13 @@
         <f t="shared" si="1"/>
         <v>2001</v>
       </c>
-      <c r="L9" s="10">
+      <c r="L9" s="10"/>
+      <c r="M9" s="10">
         <f>-J9*F9</f>
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" s="9" t="s">
         <v>10</v>
       </c>
@@ -859,8 +911,8 @@
         <v>-4890.55</v>
       </c>
       <c r="I10" s="15">
-        <f>H10-L12</f>
-        <v>6</v>
+        <f>H10-M14</f>
+        <v>-994</v>
       </c>
       <c r="J10">
         <f>IF(D10="BUY",1,-1)</f>
@@ -870,12 +922,13 @@
         <f t="shared" si="1"/>
         <v>1000</v>
       </c>
-      <c r="L10" s="10">
+      <c r="L10" s="10"/>
+      <c r="M10" s="10">
         <f>-J10*F10</f>
         <v>1000.45</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" s="9"/>
       <c r="B11" s="3"/>
       <c r="C11" s="8" t="s">
@@ -895,15 +948,37 @@
       <c r="J11" s="12">
         <v>1</v>
       </c>
-      <c r="L11" s="10">
+      <c r="M11" s="10">
         <f>-J11*F11</f>
         <v>-502</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="L12" s="10">
-        <f>SUM(L2:L11)</f>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="K12" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="L12" s="17"/>
+      <c r="M12" s="18">
+        <f>SUM(M2:M11)</f>
         <v>-4896.55</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="K13" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="M13" s="10">
+        <f>B10</f>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="K14" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="M14" s="20">
+        <f>M13+M12</f>
+        <v>-3896.55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>